<commit_message>
vhdl and new exel
</commit_message>
<xml_diff>
--- a/Excel/Dadda_tree.xlsx
+++ b/Excel/Dadda_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianl\Documents\GitHub\Dadda_tree\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0590BE55-51E1-4BB1-853C-F65F86B38A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D1A550-2D4B-4B8A-B310-3EB4552DD66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12672" yWindow="96" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="22">
   <si>
     <t>Operand</t>
   </si>
@@ -86,10 +86,19 @@
     <t>FA</t>
   </si>
   <si>
-    <t>31 bit plane adder</t>
+    <t>63 bit plane adder</t>
   </si>
   <si>
-    <t>v</t>
+    <t xml:space="preserve">NB tranne ultima riga </t>
+  </si>
+  <si>
+    <t>33 bit</t>
+  </si>
+  <si>
+    <t>Ultima riga</t>
+  </si>
+  <si>
+    <t>32 bit</t>
   </si>
 </sst>
 </file>
@@ -779,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BY72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,6 +1106,102 @@
       </c>
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1">
+        <v>60</v>
+      </c>
+      <c r="G10" s="1">
+        <v>59</v>
+      </c>
+      <c r="H10" s="1">
+        <v>58</v>
+      </c>
+      <c r="I10" s="1">
+        <v>57</v>
+      </c>
+      <c r="J10" s="1">
+        <v>56</v>
+      </c>
+      <c r="K10" s="1">
+        <v>55</v>
+      </c>
+      <c r="L10" s="1">
+        <v>54</v>
+      </c>
+      <c r="M10" s="1">
+        <v>53</v>
+      </c>
+      <c r="N10" s="1">
+        <v>52</v>
+      </c>
+      <c r="O10" s="1">
+        <v>51</v>
+      </c>
+      <c r="P10" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>49</v>
+      </c>
+      <c r="R10" s="1">
+        <v>48</v>
+      </c>
+      <c r="S10" s="1">
+        <v>47</v>
+      </c>
+      <c r="T10" s="1">
+        <v>46</v>
+      </c>
+      <c r="U10" s="1">
+        <v>45</v>
+      </c>
+      <c r="V10" s="1">
+        <v>44</v>
+      </c>
+      <c r="W10" s="1">
+        <v>43</v>
+      </c>
+      <c r="X10" s="1">
+        <v>42</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>41</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>40</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>39</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>38</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>37</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>36</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>35</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>34</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>33</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>32</v>
+      </c>
       <c r="AI10" s="1">
         <v>31</v>
       </c>
@@ -1228,7 +1333,7 @@
         <v>2</v>
       </c>
       <c r="AG12" s="37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH12" s="37" t="s">
         <v>1</v>
@@ -1815,7 +1920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>6</v>
       </c>
@@ -1840,8 +1945,8 @@
       <c r="AB17" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AC17" s="37" t="s">
-        <v>18</v>
+      <c r="AC17" s="38" t="s">
+        <v>1</v>
       </c>
       <c r="AD17" s="38" t="s">
         <v>1</v>
@@ -1928,7 +2033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>7</v>
       </c>
@@ -2041,7 +2146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>8</v>
       </c>
@@ -2153,8 +2258,14 @@
       <c r="BB19" s="16" t="s">
         <v>2</v>
       </c>
+      <c r="BT19" t="s">
+        <v>18</v>
+      </c>
+      <c r="BW19" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A20" s="17">
         <v>9</v>
       </c>
@@ -2266,8 +2377,14 @@
       <c r="AZ20" s="16" t="s">
         <v>2</v>
       </c>
+      <c r="BT20" t="s">
+        <v>20</v>
+      </c>
+      <c r="BW20" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>10</v>
       </c>
@@ -2380,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>11</v>
       </c>
@@ -2493,7 +2610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>12</v>
       </c>
@@ -2606,7 +2723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>13</v>
       </c>
@@ -2719,7 +2836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>14</v>
       </c>
@@ -2832,7 +2949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>15</v>
       </c>
@@ -2946,7 +3063,7 @@
       </c>
       <c r="BO26" s="13"/>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>16</v>
       </c>
@@ -3057,7 +3174,7 @@
       </c>
       <c r="BO27" s="13"/>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>17</v>
       </c>
@@ -3162,7 +3279,7 @@
       </c>
       <c r="BO28" s="13"/>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
       <c r="B29" s="23"/>
       <c r="C29" s="24"/>
@@ -3237,7 +3354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>1</v>
       </c>
@@ -3438,7 +3555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>2</v>
       </c>
@@ -3633,7 +3750,7 @@
       </c>
       <c r="BO31" s="13"/>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>3</v>
       </c>

</xml_diff>